<commit_message>
adding short strategy with PMI
</commit_message>
<xml_diff>
--- a/tvix_night_outlier_noted.xlsx
+++ b/tvix_night_outlier_noted.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junyan/Desktop/TVIX/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="24320" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -250,6 +255,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -541,13 +551,13 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9" ySplit="22" topLeftCell="J27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="22" topLeftCell="K23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
+      <selection pane="bottomRight" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
@@ -557,7 +567,7 @@
     <col min="14" max="14" width="53.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40616</v>
       </c>
@@ -645,7 +655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>40716</v>
       </c>
@@ -686,7 +696,7 @@
         <v>-0.12938329430132711</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>40760</v>
       </c>
@@ -730,7 +740,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>40772</v>
       </c>
@@ -771,7 +781,7 @@
         <v>-3.3970810266733771E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>40773</v>
       </c>
@@ -812,7 +822,7 @@
         <v>0.52828054298642535</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>40788</v>
       </c>
@@ -853,7 +863,7 @@
         <v>0.1318968989126057</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>40807</v>
       </c>
@@ -894,7 +904,7 @@
         <v>0.1799675734101964</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>40847</v>
       </c>
@@ -935,7 +945,7 @@
         <v>-0.1155269822715761</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>40855</v>
       </c>
@@ -976,7 +986,7 @@
         <v>-7.3082343466881416E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>40865</v>
       </c>
@@ -1017,7 +1027,7 @@
         <v>0.12543285879184299</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>40948</v>
       </c>
@@ -1058,7 +1068,7 @@
         <v>0.16870064608758081</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>40996</v>
       </c>
@@ -1099,7 +1109,7 @@
         <v>4.1899441340782122E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>41004</v>
       </c>
@@ -1140,7 +1150,7 @@
         <v>9.2329545454545456E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>41060</v>
       </c>
@@ -1181,7 +1191,7 @@
         <v>4.4724770642201837E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>41110</v>
       </c>
@@ -1222,7 +1232,7 @@
         <v>6.8535825545171333E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>41204</v>
       </c>
@@ -1263,7 +1273,7 @@
         <v>5.3846153846153849E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>41446</v>
       </c>
@@ -1304,7 +1314,7 @@
         <v>0.12871287128712869</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>41669</v>
       </c>
@@ -1345,7 +1355,7 @@
         <v>4.8959608323133411E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>41698</v>
       </c>
@@ -1386,7 +1396,7 @@
         <v>4.9928673323823107E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>41829</v>
       </c>
@@ -1427,7 +1437,7 @@
         <v>3.3457249070631967E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>41926</v>
       </c>
@@ -1468,7 +1478,7 @@
         <v>0.42388059701492542</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>41927</v>
       </c>
@@ -1509,7 +1519,7 @@
         <v>0.1844660194174757</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>42181</v>
       </c>
@@ -1550,7 +1560,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>42227</v>
       </c>
@@ -1591,7 +1601,7 @@
         <v>-1.6977928692699491E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>42236</v>
       </c>
@@ -1632,7 +1642,7 @@
         <v>0.24545454545454551</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>42237</v>
       </c>
@@ -1673,7 +1683,7 @@
         <v>0.62588652482269502</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>42247</v>
       </c>
@@ -1714,7 +1724,7 @@
         <v>0.23785594639866001</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>42264</v>
       </c>
@@ -1755,7 +1765,7 @@
         <v>-0.3017306245297216</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>42348</v>
       </c>
@@ -1796,7 +1806,7 @@
         <v>0.16637781629116119</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>42369</v>
       </c>
@@ -1840,7 +1850,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>42374</v>
       </c>
@@ -1884,7 +1894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>42375</v>
       </c>
@@ -1928,7 +1938,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>42383</v>
       </c>
@@ -1972,7 +1982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>42410</v>
       </c>
@@ -2016,7 +2026,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>42544</v>
       </c>
@@ -2060,7 +2070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>42682</v>
       </c>
@@ -2104,7 +2114,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>42871</v>
       </c>
@@ -2151,10 +2161,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>